<commit_message>
change the files that make the program scnycroned with all the files , which update the data from the user to be inside the relvant place
</commit_message>
<xml_diff>
--- a/SearchOption1/Emails-List.xlsx
+++ b/SearchOption1/Emails-List.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Company Name</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>2023-31-21 11:31:43</t>
+  </si>
+  <si>
+    <t>2023-01-27 02:01:03</t>
+  </si>
+  <si>
+    <t>2023-13-29 02:13:51</t>
   </si>
 </sst>
 </file>
@@ -559,8 +565,12 @@
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -570,8 +580,12 @@
         <v>9</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -581,8 +595,12 @@
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -592,8 +610,12 @@
         <v>11</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -603,8 +625,12 @@
         <v>12</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -614,8 +640,12 @@
         <v>13</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">

</xml_diff>